<commit_message>
Agregando graficos de excel
</commit_message>
<xml_diff>
--- a/MedicionesAD736v2.xlsx
+++ b/MedicionesAD736v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\TPO-MEI-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E214E86-E12A-4957-8BC2-CE985CB90357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5ADCA0-BC28-4B0A-B165-B287E979A1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2452281E-B86C-4117-B9C7-7620DA804AAA}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vi</t>
   </si>
   <si>
     <t>Vv</t>
-  </si>
-  <si>
-    <t>5.05</t>
   </si>
   <si>
     <t>Frecuencia</t>
@@ -104,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -138,11 +135,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,10 +162,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,7 +238,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3136482939632545E-2"/>
+          <c:y val="0.16708333333333336"/>
+          <c:w val="0.87119685039370076"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -679,7 +708,1142 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.85219685039370074"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medicion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>86.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>100.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>101.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>101.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>101.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>101.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>100.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100.1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>99.8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>92.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>85.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>74.099999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-947E-4293-85E2-FBFFC087210F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2094128959"/>
+        <c:axId val="1449355423"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2094128959"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1449355423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1449355423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094128959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2125963559915915E-2"/>
+          <c:y val="0.15110952746084175"/>
+          <c:w val="0.87103889278206026"/>
+          <c:h val="0.71610683558496757"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-419"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>105.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7E9-4EA9-BC43-C117FA15E690}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2096836159"/>
+        <c:axId val="2043158415"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2096836159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2043158415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2043158415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2096836159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1235,6 +2399,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1268,6 +3464,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>596348</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB1E27FC-0A26-5C1A-36E4-713E38D849E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>538394</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>111197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>339611</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>71440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51651453-AE06-11BC-D9F1-0DFC3497F608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1575,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D51AC8-B761-43DE-AFAC-69E6BC586A37}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,41 +3853,41 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.0580000000000001</v>
-      </c>
-      <c r="C2" s="5">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
-        <v>11.5</v>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10.4</v>
       </c>
       <c r="E2">
-        <f>D2-1.4</f>
-        <v>10.1</v>
+        <f>D2-1.6</f>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F2" s="4">
         <v>11.8</v>
@@ -1630,20 +3898,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>6.3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>27.7</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>21.7</v>
+      <c r="D3" s="4">
+        <v>11.9</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E47" si="0">D3-1.4</f>
-        <v>20.3</v>
+        <f t="shared" ref="E3:E47" si="0">D3-1.6</f>
+        <v>10.3</v>
       </c>
       <c r="F3" s="4">
         <v>12.9</v>
@@ -1654,20 +3922,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>9.77</v>
-      </c>
-      <c r="C4" s="5">
+        <v>28.6</v>
+      </c>
+      <c r="B4" s="8">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
-        <v>33.5</v>
+      <c r="D4" s="4">
+        <v>15.2</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>32.1</v>
+        <v>13.6</v>
       </c>
       <c r="F4" s="4">
         <v>15.7</v>
@@ -1678,20 +3946,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>21.4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>19.48</v>
-      </c>
-      <c r="C5" s="5">
+        <v>30.8</v>
+      </c>
+      <c r="B5" s="8">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="5">
-        <v>46.1</v>
+      <c r="D5" s="4">
+        <v>19.5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>44.7</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="F5" s="4">
         <v>19.5</v>
@@ -1702,20 +3970,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>31.5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>29.2</v>
-      </c>
-      <c r="C6" s="5">
+        <v>36.9</v>
+      </c>
+      <c r="B6" s="8">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
-        <v>57.8</v>
+      <c r="D6" s="4">
+        <v>24.3</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>56.4</v>
+        <v>22.7</v>
       </c>
       <c r="F6" s="4">
         <v>23.8</v>
@@ -1726,20 +3994,20 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>42.1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>39.020000000000003</v>
-      </c>
-      <c r="C7" s="5">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="B7" s="8">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="5">
-        <v>68.8</v>
+      <c r="D7" s="4">
+        <v>29.2</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>67.399999999999991</v>
+        <v>27.599999999999998</v>
       </c>
       <c r="F7" s="4">
         <v>28.3</v>
@@ -1750,20 +4018,20 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>52.1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>48.76</v>
-      </c>
-      <c r="C8" s="5">
+        <v>44.8</v>
+      </c>
+      <c r="B8" s="8">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D8" s="5">
-        <v>78.900000000000006</v>
+      <c r="D8" s="4">
+        <v>34.4</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>77.5</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F8" s="4">
         <v>33</v>
@@ -1774,20 +4042,20 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="B9" s="2">
-        <v>60.48</v>
-      </c>
-      <c r="C9" s="5">
+        <v>49</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="5">
-        <v>88.4</v>
+      <c r="D9" s="4">
+        <v>39</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>37.4</v>
       </c>
       <c r="F9" s="4">
         <v>37.9</v>
@@ -1798,20 +4066,20 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="B10" s="2">
-        <v>70.12</v>
-      </c>
-      <c r="C10" s="5">
+        <v>53.4</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4">
         <v>9</v>
       </c>
-      <c r="D10" s="5">
-        <v>97.2</v>
+      <c r="D10" s="4">
+        <v>43.5</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>95.8</v>
+        <v>41.9</v>
       </c>
       <c r="F10" s="4">
         <v>43.3</v>
@@ -1822,20 +4090,20 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>85.5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>80.7</v>
-      </c>
-      <c r="C11" s="5">
+        <v>57.9</v>
+      </c>
+      <c r="B11" s="8">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4">
         <v>10</v>
       </c>
-      <c r="D11" s="5">
-        <v>107.7</v>
+      <c r="D11" s="4">
+        <v>47.6</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>106.3</v>
+        <v>46</v>
       </c>
       <c r="F11" s="4">
         <v>48.3</v>
@@ -1846,20 +4114,20 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>95.3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>90.38</v>
-      </c>
-      <c r="C12" s="5">
+        <v>62.5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4">
         <v>20</v>
       </c>
-      <c r="D12" s="5">
-        <v>158.4</v>
+      <c r="D12" s="4">
+        <v>74.8</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>157</v>
+        <v>73.2</v>
       </c>
       <c r="F12" s="4">
         <v>56.3</v>
@@ -1870,20 +4138,20 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>106.2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>100.86</v>
-      </c>
-      <c r="C13" s="5">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="B13" s="8">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4">
         <v>30</v>
       </c>
-      <c r="D13" s="5">
-        <v>179.1</v>
+      <c r="D13" s="4">
+        <v>86.1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>177.7</v>
+        <v>84.5</v>
       </c>
       <c r="F13" s="4">
         <v>63.3</v>
@@ -1894,20 +4162,20 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>116.6</v>
-      </c>
-      <c r="B14" s="2">
-        <v>110.58</v>
-      </c>
-      <c r="C14" s="5">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="B14" s="8">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4">
         <v>40</v>
       </c>
-      <c r="D14" s="5">
-        <v>188.5</v>
+      <c r="D14" s="4">
+        <v>91.2</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>187.1</v>
+        <v>89.600000000000009</v>
       </c>
       <c r="F14" s="4">
         <v>73.400000000000006</v>
@@ -1918,20 +4186,20 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>127.6</v>
-      </c>
-      <c r="B15" s="2">
-        <v>121.07</v>
-      </c>
-      <c r="C15" s="5">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="B15" s="8">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4">
         <v>50</v>
       </c>
-      <c r="D15" s="5">
-        <v>190</v>
+      <c r="D15" s="4">
+        <v>92.5</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>188.6</v>
+        <v>90.9</v>
       </c>
       <c r="F15" s="4">
         <v>83.4</v>
@@ -1942,20 +4210,20 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>137.19999999999999</v>
-      </c>
-      <c r="B16" s="2">
-        <v>130.72999999999999</v>
-      </c>
-      <c r="C16" s="5">
+        <v>86.2</v>
+      </c>
+      <c r="B16" s="8">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4">
         <v>60</v>
       </c>
-      <c r="D16" s="5">
-        <v>193.9</v>
+      <c r="D16" s="4">
+        <v>95.5</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>192.5</v>
+        <v>93.9</v>
       </c>
       <c r="F16" s="4">
         <v>93.7</v>
@@ -1966,20 +4234,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>148.30000000000001</v>
-      </c>
-      <c r="B17" s="2">
-        <v>141.22</v>
-      </c>
-      <c r="C17" s="5">
+        <v>91</v>
+      </c>
+      <c r="B17" s="8">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4">
         <v>70</v>
       </c>
-      <c r="D17" s="5">
-        <v>195.8</v>
+      <c r="D17" s="4">
+        <v>96.8</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>194.4</v>
+        <v>95.2</v>
       </c>
       <c r="F17" s="4">
         <v>103.9</v>
@@ -1990,20 +4258,20 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>158.6</v>
-      </c>
-      <c r="B18" s="2">
-        <v>150.91999999999999</v>
-      </c>
-      <c r="C18" s="5">
+        <v>96</v>
+      </c>
+      <c r="B18" s="8">
+        <v>90</v>
+      </c>
+      <c r="C18" s="4">
         <v>80</v>
       </c>
-      <c r="D18" s="5">
-        <v>197</v>
+      <c r="D18" s="4">
+        <v>97.3</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>195.6</v>
+        <v>95.7</v>
       </c>
       <c r="F18" s="4">
         <v>114</v>
@@ -2014,20 +4282,20 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>169.2</v>
-      </c>
-      <c r="B19" s="2">
-        <v>161.44</v>
-      </c>
-      <c r="C19" s="5">
+        <v>100.9</v>
+      </c>
+      <c r="B19" s="8">
+        <v>95</v>
+      </c>
+      <c r="C19" s="4">
         <v>90</v>
       </c>
-      <c r="D19" s="5">
-        <v>197.8</v>
+      <c r="D19" s="4">
+        <v>97.8</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>196.4</v>
+        <v>96.2</v>
       </c>
       <c r="F19" s="4">
         <v>124.2</v>
@@ -2038,20 +4306,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>179.1</v>
-      </c>
-      <c r="B20" s="2">
-        <v>171.08</v>
-      </c>
-      <c r="C20" s="5">
+        <v>105.7</v>
+      </c>
+      <c r="B20" s="8">
         <v>100</v>
       </c>
-      <c r="D20" s="5">
-        <v>198.3</v>
+      <c r="C20" s="4">
+        <v>100</v>
+      </c>
+      <c r="D20" s="4">
+        <v>98.5</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>196.9</v>
+        <v>96.9</v>
       </c>
       <c r="F20" s="4">
         <v>134.30000000000001</v>
@@ -2061,21 +4329,17 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>190</v>
-      </c>
-      <c r="B21" s="2">
-        <v>181.61</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="4">
         <v>200</v>
       </c>
-      <c r="D21" s="5">
-        <v>200.6</v>
+      <c r="D21" s="4">
+        <v>100.3</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>199.2</v>
+        <v>98.7</v>
       </c>
       <c r="F21" s="4">
         <v>144.5</v>
@@ -2085,21 +4349,17 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>200.2</v>
-      </c>
-      <c r="B22" s="2">
-        <v>191.25</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="4">
         <v>300</v>
       </c>
-      <c r="D22" s="5">
-        <v>201.1</v>
+      <c r="D22" s="4">
+        <v>100.6</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>199.7</v>
+        <v>99</v>
       </c>
       <c r="F22" s="4">
         <v>154.69999999999999</v>
@@ -2109,21 +4369,17 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>211.1</v>
-      </c>
-      <c r="B23" s="2">
-        <v>201.82</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4">
         <v>400</v>
       </c>
-      <c r="D23" s="5">
-        <v>201.2</v>
+      <c r="D23" s="4">
+        <v>100.5</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>199.79999999999998</v>
+        <v>98.9</v>
       </c>
       <c r="F23" s="4">
         <v>164.9</v>
@@ -2133,15 +4389,15 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>500</v>
       </c>
-      <c r="D24" s="5">
-        <v>201.3</v>
+      <c r="D24" s="4">
+        <v>100.7</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>199.9</v>
+        <v>99.100000000000009</v>
       </c>
       <c r="F24" s="4">
         <v>175</v>
@@ -2151,15 +4407,16 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="5">
+      <c r="B25" s="9"/>
+      <c r="C25" s="4">
         <v>600</v>
       </c>
-      <c r="D25" s="5">
-        <v>201.4</v>
+      <c r="D25" s="4">
+        <v>100.7</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.100000000000009</v>
       </c>
       <c r="F25" s="4">
         <v>185.1</v>
@@ -2169,15 +4426,15 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>700</v>
       </c>
-      <c r="D26" s="5">
-        <v>201.4</v>
+      <c r="D26" s="4">
+        <v>101.4</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.800000000000011</v>
       </c>
       <c r="F26" s="4">
         <v>195.1</v>
@@ -2187,15 +4444,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>800</v>
       </c>
-      <c r="D27" s="5">
-        <v>201.4</v>
+      <c r="D27" s="4">
+        <v>101.5</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.9</v>
       </c>
       <c r="F27" s="4">
         <v>205.2</v>
@@ -2205,243 +4462,243 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>900</v>
       </c>
-      <c r="D28" s="5">
-        <v>201.4</v>
+      <c r="D28" s="4">
+        <v>101.6</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>1000</v>
       </c>
-      <c r="D29" s="5">
-        <v>201.4</v>
+      <c r="D29" s="4">
+        <v>101.1</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>2000</v>
       </c>
-      <c r="D30" s="5">
-        <v>201.4</v>
+      <c r="D30" s="4">
+        <v>100.9</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.300000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>3000</v>
       </c>
-      <c r="D31" s="5">
-        <v>201.4</v>
+      <c r="D31" s="4">
+        <v>100.9</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>99.300000000000011</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>4000</v>
       </c>
-      <c r="D32" s="5">
-        <v>201.3</v>
+      <c r="D32" s="4">
+        <v>100.9</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>199.9</v>
+        <v>99.300000000000011</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>5000</v>
       </c>
-      <c r="D33" s="5">
-        <v>201.2</v>
+      <c r="D33" s="4">
+        <v>100.8</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>199.79999999999998</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>6000</v>
       </c>
-      <c r="D34" s="5">
-        <v>201.1</v>
+      <c r="D34" s="4">
+        <v>100.6</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>199.7</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>7000</v>
       </c>
-      <c r="D35" s="5">
-        <v>201</v>
+      <c r="D35" s="4">
+        <v>100.3</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>199.6</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>8000</v>
       </c>
-      <c r="D36" s="5">
-        <v>200.7</v>
+      <c r="D36" s="4">
+        <v>100.1</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>199.29999999999998</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>9000</v>
       </c>
-      <c r="D37" s="5">
-        <v>200.6</v>
+      <c r="D37" s="4">
+        <v>100</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>199.2</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C38" s="5">
+      <c r="C38" s="4">
         <v>10000</v>
       </c>
-      <c r="D38" s="5">
-        <v>200.4</v>
+      <c r="D38" s="4">
+        <v>99.8</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>20000</v>
       </c>
-      <c r="D39" s="5">
-        <v>197.7</v>
+      <c r="D39" s="4">
+        <v>98</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>196.29999999999998</v>
+        <v>96.4</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>30000</v>
       </c>
-      <c r="D40" s="5">
-        <v>193.8</v>
+      <c r="D40" s="4">
+        <v>95.7</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>192.4</v>
+        <v>94.100000000000009</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>40000</v>
       </c>
-      <c r="D41" s="5">
-        <v>188.9</v>
+      <c r="D41" s="4">
+        <v>92.8</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>187.5</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>50000</v>
       </c>
-      <c r="D42" s="5">
-        <v>183.5</v>
+      <c r="D42" s="4">
+        <v>90.1</v>
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>182.1</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>60000</v>
       </c>
-      <c r="D43" s="5">
-        <v>177.8</v>
+      <c r="D43" s="4">
+        <v>85.9</v>
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>176.4</v>
+        <v>84.300000000000011</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>70000</v>
       </c>
-      <c r="D44" s="5">
-        <v>172.4</v>
+      <c r="D44" s="4">
+        <v>82.8</v>
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>81.2</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C45" s="5">
+      <c r="C45" s="4">
         <v>80000</v>
       </c>
-      <c r="D45" s="5">
-        <v>167.4</v>
+      <c r="D45" s="4">
+        <v>79.5</v>
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>77.900000000000006</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>90000</v>
       </c>
-      <c r="D46" s="5">
-        <v>162.5</v>
+      <c r="D46" s="4">
+        <v>76.5</v>
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
-        <v>161.1</v>
+        <v>74.900000000000006</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>100000</v>
       </c>
-      <c r="D47" s="5">
-        <v>158.9</v>
+      <c r="D47" s="4">
+        <v>74.099999999999994</v>
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
-        <v>157.5</v>
+        <v>72.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>